<commit_message>
small adaptions to the ArcGIS import
</commit_message>
<xml_diff>
--- a/ModellingToolbox/tests/test_data/Random_Data.xlsx
+++ b/ModellingToolbox/tests/test_data/Random_Data.xlsx
@@ -149,12 +149,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -474,22 +480,23 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H7" sqref="H6:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="13.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="13.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="16384" width="13.140625" style="2"/>
+    <col min="1" max="3" width="13.1328125" style="4"/>
+    <col min="4" max="16384" width="13.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -508,166 +515,166 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="4">
         <f ca="1">RANDBETWEEN(4450000,4550000)+RAND()</f>
-        <v>4477448.4834189313</v>
-      </c>
-      <c r="B2" s="2">
+        <v>4485451.0185431205</v>
+      </c>
+      <c r="B2" s="4">
         <f ca="1">RANDBETWEEN(5640000,5660000)+RAND()</f>
-        <v>5651380.7409052551</v>
-      </c>
-      <c r="C2" s="2">
+        <v>5647776.0780213643</v>
+      </c>
+      <c r="C2" s="4">
         <f ca="1">RANDBETWEEN(100,500)+RAND()</f>
-        <v>429.18750816717477</v>
+        <v>444.48101867347214</v>
       </c>
       <c r="D2" s="2">
         <f ca="1">RANDBETWEEN(2,20)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D2,1)</f>
-        <v>ku</v>
+        <v>ko</v>
       </c>
       <c r="F2" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D2,2)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G2" s="2" t="str">
         <f ca="1">IF(RANDBETWEEN(1,2)=1,"Point Set","")</f>
-        <v/>
+        <v>Point Set</v>
       </c>
       <c r="H2" s="2" t="str">
         <f ca="1">IF(RANDBETWEEN(1,1000)&gt;500,RANDBETWEEN(501,1000),"")</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="4">
         <f t="shared" ref="A3:A40" ca="1" si="0">RANDBETWEEN(4450000,4550000)+RAND()</f>
-        <v>4475387.3284328422</v>
-      </c>
-      <c r="B3" s="2">
+        <v>4467210.0793929957</v>
+      </c>
+      <c r="B3" s="4">
         <f t="shared" ref="B3:B40" ca="1" si="1">RANDBETWEEN(5640000,5660000)+RAND()</f>
-        <v>5649850.1004939685</v>
-      </c>
-      <c r="C3" s="2">
+        <v>5654330.0560828168</v>
+      </c>
+      <c r="C3" s="4">
         <f t="shared" ref="C3:C40" ca="1" si="2">RANDBETWEEN(100,500)+RAND()</f>
-        <v>296.39104759676275</v>
+        <v>291.45870913268197</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D40" ca="1" si="3">RANDBETWEEN(2,20)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D3,1)</f>
-        <v>t</v>
+        <v>mo</v>
       </c>
       <c r="F3" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D3,2)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G3" s="2" t="str">
         <f t="shared" ref="G3:G40" ca="1" si="4">IF(RANDBETWEEN(1,2)=1,"Point Set","")</f>
-        <v>Point Set</v>
-      </c>
-      <c r="H3" s="2" t="str">
+        <v/>
+      </c>
+      <c r="H3" s="2">
         <f t="shared" ref="H3:H40" ca="1" si="5">IF(RANDBETWEEN(1,1000)&gt;500,RANDBETWEEN(501,1000),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4462935.2136923084</v>
-      </c>
-      <c r="B4" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5647218.5086331749</v>
-      </c>
-      <c r="C4" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>295.65520153557128</v>
+        <v>568</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4493066.4215491172</v>
+      </c>
+      <c r="B4" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5649436.3620075928</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>442.46138007676308</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D4,1)</f>
-        <v>ko</v>
+        <v>c</v>
       </c>
       <c r="F4" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D4,2)</f>
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G4" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Point Set</v>
+        <v/>
       </c>
       <c r="H4" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>524</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4528063.9684534026</v>
-      </c>
-      <c r="B5" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5650422.3164768284</v>
-      </c>
-      <c r="C5" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>129.71690214090484</v>
+        <v>836</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4456841.252703391</v>
+      </c>
+      <c r="B5" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5655594.6898874389</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>145.35272289742355</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E5" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D5,1)</f>
-        <v>c</v>
+        <v>q</v>
       </c>
       <c r="F5" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D5,2)</f>
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="G5" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
         <v>Point Set</v>
       </c>
-      <c r="H5" s="2" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4505559.0159101412</v>
-      </c>
-      <c r="B6" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5641646.5664453395</v>
-      </c>
-      <c r="C6" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>149.71860612030937</v>
+      <c r="H5" s="2">
+        <f t="shared" ca="1" si="5"/>
+        <v>940</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4480470.490249834</v>
+      </c>
+      <c r="B6" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5654369.0207953416</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>169.89996259415506</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D6,1)</f>
-        <v>ru</v>
+        <v>mo</v>
       </c>
       <c r="F6" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D6,2)</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G6" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -678,30 +685,30 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4536624.5807693619</v>
-      </c>
-      <c r="B7" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5657927.0676580556</v>
-      </c>
-      <c r="C7" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>333.4662554669838</v>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4474727.5103825433</v>
+      </c>
+      <c r="B7" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5643683.0330507113</v>
+      </c>
+      <c r="C7" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>443.34898048448343</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E7" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D7,1)</f>
-        <v>mo</v>
+        <v>ko</v>
       </c>
       <c r="F7" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D7,2)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G7" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -709,67 +716,67 @@
       </c>
       <c r="H7" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>507</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4496481.2679857574</v>
-      </c>
-      <c r="B8" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5643864.0229363814</v>
-      </c>
-      <c r="C8" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>187.49329317299475</v>
+        <v>656</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4502699.3062865296</v>
+      </c>
+      <c r="B8" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5659135.1192646921</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>125.99842186959197</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E8" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D8,1)</f>
-        <v>t</v>
+        <v>sm</v>
       </c>
       <c r="F8" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D8,2)</f>
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G8" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Point Set</v>
-      </c>
-      <c r="H8" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>903</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4540665.0009243786</v>
-      </c>
-      <c r="B9" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5641175.6198386112</v>
-      </c>
-      <c r="C9" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>139.24174611167649</v>
+        <v/>
+      </c>
+      <c r="H8" s="2" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4543973.5939319963</v>
+      </c>
+      <c r="B9" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5656903.6841395497</v>
+      </c>
+      <c r="C9" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>464.3749276661847</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E9" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D9,1)</f>
-        <v>d</v>
+        <v>ru</v>
       </c>
       <c r="F9" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D9,2)</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G9" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -777,33 +784,33 @@
       </c>
       <c r="H9" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>708</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4488787.3439278062</v>
-      </c>
-      <c r="B10" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5644221.691205469</v>
-      </c>
-      <c r="C10" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>321.13391729145923</v>
+        <v>859</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4517098.886825298</v>
+      </c>
+      <c r="B10" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5658365.9642062588</v>
+      </c>
+      <c r="C10" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>446.50334059754306</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="E10" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D10,1)</f>
-        <v>km</v>
+        <v>ru</v>
       </c>
       <c r="F10" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D10,2)</f>
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="G10" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -814,98 +821,98 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4494893.4431548994</v>
-      </c>
-      <c r="B11" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5647718.1848827442</v>
-      </c>
-      <c r="C11" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>132.5662220770657</v>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4469134.9330846816</v>
+      </c>
+      <c r="B11" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5657547.2734332774</v>
+      </c>
+      <c r="C11" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>181.18790262703905</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E11" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D11,1)</f>
-        <v>su</v>
+        <v>q</v>
       </c>
       <c r="F11" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D11,2)</f>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G11" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="H11" s="2" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4527127.6532316972</v>
-      </c>
-      <c r="B12" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5650523.9948403602</v>
-      </c>
-      <c r="C12" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>377.66179596948592</v>
+      <c r="H11" s="2">
+        <f t="shared" ca="1" si="5"/>
+        <v>816</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4548838.422641308</v>
+      </c>
+      <c r="B12" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5647553.6749021076</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>303.21011754321455</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E12" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D12,1)</f>
-        <v>d</v>
+        <v>si</v>
       </c>
       <c r="F12" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D12,2)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G12" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
         <v>Point Set</v>
       </c>
-      <c r="H12" s="2" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4482471.8909069235</v>
-      </c>
-      <c r="B13" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5641862.5949604744</v>
-      </c>
-      <c r="C13" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>125.29613978595302</v>
+      <c r="H12" s="2">
+        <f t="shared" ca="1" si="5"/>
+        <v>726</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4549327.936412476</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5655947.1981512178</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>206.9167437242601</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E13" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D13,1)</f>
-        <v>q</v>
+        <v>t</v>
       </c>
       <c r="F13" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D13,2)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -913,33 +920,33 @@
       </c>
       <c r="H13" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>614</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4518940.959905332</v>
-      </c>
-      <c r="B14" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5646691.3770625582</v>
-      </c>
-      <c r="C14" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>445.39860762218188</v>
+        <v>712</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4471900.5856496971</v>
+      </c>
+      <c r="B14" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5643759.389377174</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>361.43961782843411</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E14" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D14,1)</f>
-        <v>d</v>
+        <v>km</v>
       </c>
       <c r="F14" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D14,2)</f>
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G14" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -947,67 +954,67 @@
       </c>
       <c r="H14" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>718</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4533280.1115813283</v>
-      </c>
-      <c r="B15" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5642831.42322753</v>
-      </c>
-      <c r="C15" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>480.01533344443027</v>
+        <v>742</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4503267.1741625797</v>
+      </c>
+      <c r="B15" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5649799.1855851328</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>249.19307532277926</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E15" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D15,1)</f>
-        <v>ku</v>
+        <v>ru</v>
       </c>
       <c r="F15" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D15,2)</f>
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="G15" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
         <v>Point Set</v>
       </c>
-      <c r="H15" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>720</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4465606.0465486366</v>
-      </c>
-      <c r="B16" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5657925.40934618</v>
-      </c>
-      <c r="C16" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>351.89437959588065</v>
+      <c r="H15" s="2" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4536292.7956593186</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5645696.0392396925</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>224.05858304909026</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E16" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D16,1)</f>
-        <v>mo</v>
+        <v>d</v>
       </c>
       <c r="F16" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D16,2)</f>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="G16" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -1015,135 +1022,135 @@
       </c>
       <c r="H16" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>841</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4549822.3773545586</v>
-      </c>
-      <c r="B17" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5645321.7310677757</v>
-      </c>
-      <c r="C17" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>223.61288243504922</v>
+        <v>909</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4511057.6238211375</v>
+      </c>
+      <c r="B17" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5655307.2930335188</v>
+      </c>
+      <c r="C17" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>143.49637125146722</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E17" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D17,1)</f>
-        <v>d</v>
+        <v>mm</v>
       </c>
       <c r="F17" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D17,2)</f>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="G17" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
         <v>Point Set</v>
       </c>
-      <c r="H17" s="2" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4484083.1098495023</v>
-      </c>
-      <c r="B18" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5642257.7283544326</v>
-      </c>
-      <c r="C18" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>213.40123013392278</v>
+      <c r="H17" s="2">
+        <f t="shared" ca="1" si="5"/>
+        <v>645</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4522632.3086177111</v>
+      </c>
+      <c r="B18" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5650407.2388213035</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>220.44360844089826</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E18" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D18,1)</f>
-        <v>mo</v>
+        <v>mu</v>
       </c>
       <c r="F18" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D18,2)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G18" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Point Set</v>
+        <v/>
       </c>
       <c r="H18" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4533582.1299095573</v>
-      </c>
-      <c r="B19" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5659393.5482848166</v>
-      </c>
-      <c r="C19" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>115.77966117515325</v>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4456117.5900531486</v>
+      </c>
+      <c r="B19" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5650661.8706419403</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>258.90233226037304</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E19" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D19,1)</f>
-        <v>su</v>
+        <v>km</v>
       </c>
       <c r="F19" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D19,2)</f>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G19" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="H19" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4498345.0124912597</v>
-      </c>
-      <c r="B20" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5650419.062893549</v>
-      </c>
-      <c r="C20" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>365.4220844137655</v>
+      <c r="H19" s="2" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4533498.5888456758</v>
+      </c>
+      <c r="B20" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5656985.5861155828</v>
+      </c>
+      <c r="C20" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>140.57910601902717</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E20" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D20,1)</f>
-        <v>z</v>
+        <v>so</v>
       </c>
       <c r="F20" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D20,2)</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G20" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -1154,86 +1161,86 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4513113.0943259383</v>
-      </c>
-      <c r="B21" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5646245.9370920714</v>
-      </c>
-      <c r="C21" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>221.24652851405682</v>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4523911.7941731652</v>
+      </c>
+      <c r="B21" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5645888.995473858</v>
+      </c>
+      <c r="C21" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>377.14109887909842</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E21" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D21,1)</f>
-        <v>kr</v>
+        <v>mu</v>
       </c>
       <c r="F21" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D21,2)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G21" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Point Set</v>
-      </c>
-      <c r="H21" s="2" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4468922.0518670231</v>
-      </c>
-      <c r="B22" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5646091.0563950511</v>
-      </c>
-      <c r="C22" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>251.13738027442727</v>
+        <v/>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" ca="1" si="5"/>
+        <v>763</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4498253.5595818199</v>
+      </c>
+      <c r="B22" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5650483.3962306408</v>
+      </c>
+      <c r="C22" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>216.36365612542397</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E22" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D22,1)</f>
-        <v>km</v>
+        <v>mu</v>
       </c>
       <c r="F22" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D22,2)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G22" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="H22" s="2" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4503451.6680079121</v>
-      </c>
-      <c r="B23" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5641637.9516896894</v>
-      </c>
-      <c r="C23" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>330.22986672897889</v>
+        <v>Point Set</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" ca="1" si="5"/>
+        <v>515</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4545110.8254473424</v>
+      </c>
+      <c r="B23" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5659629.3183471644</v>
+      </c>
+      <c r="C23" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>139.08056799744497</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" ca="1" si="3"/>
@@ -1251,91 +1258,91 @@
         <f t="shared" ca="1" si="4"/>
         <v>Point Set</v>
       </c>
-      <c r="H23" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>729</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4516157.5632426171</v>
-      </c>
-      <c r="B24" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5650931.3050880888</v>
-      </c>
-      <c r="C24" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>267.53759813743238</v>
+      <c r="H23" s="2" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4481328.4127359809</v>
+      </c>
+      <c r="B24" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5658730.4944530781</v>
+      </c>
+      <c r="C24" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>124.08741331928925</v>
       </c>
       <c r="D24" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E24" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D24,1)</f>
-        <v>si</v>
+        <v>ro</v>
       </c>
       <c r="F24" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D24,2)</f>
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G24" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="H24" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>734</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4523721.76641024</v>
-      </c>
-      <c r="B25" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5645314.1354359649</v>
-      </c>
-      <c r="C25" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>142.32907164927425</v>
+        <v>Point Set</v>
+      </c>
+      <c r="H24" s="2" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4494026.0144406529</v>
+      </c>
+      <c r="B25" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5654556.7507177358</v>
+      </c>
+      <c r="C25" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>173.08656684375595</v>
       </c>
       <c r="D25" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E25" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D25,1)</f>
-        <v>ko</v>
+        <v>km</v>
       </c>
       <c r="F25" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D25,2)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G25" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
-      </c>
-      <c r="H25" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>843</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4546143.0135550164</v>
-      </c>
-      <c r="B26" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5645098.3589714365</v>
-      </c>
-      <c r="C26" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>487.43695914099828</v>
+        <v>Point Set</v>
+      </c>
+      <c r="H25" s="2" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A26" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4489122.5443633841</v>
+      </c>
+      <c r="B26" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5646983.9072804879</v>
+      </c>
+      <c r="C26" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>256.05974040297787</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" ca="1" si="3"/>
@@ -1355,67 +1362,67 @@
       </c>
       <c r="H26" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>843</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4484070.0553342979</v>
-      </c>
-      <c r="B27" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5656917.9646312231</v>
-      </c>
-      <c r="C27" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>455.74156212467</v>
+        <v>899</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A27" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4532801.4311805852</v>
+      </c>
+      <c r="B27" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5656404.909907531</v>
+      </c>
+      <c r="C27" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>198.53474924780096</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E27" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D27,1)</f>
-        <v>km</v>
+        <v>t</v>
       </c>
       <c r="F27" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D27,2)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G27" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Point Set</v>
-      </c>
-      <c r="H27" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>694</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4546113.784151895</v>
-      </c>
-      <c r="B28" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5655774.5114442017</v>
-      </c>
-      <c r="C28" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>232.78640153276277</v>
+        <v/>
+      </c>
+      <c r="H27" s="2" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A28" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4512128.9798038984</v>
+      </c>
+      <c r="B28" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5653580.0685498007</v>
+      </c>
+      <c r="C28" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>313.34531238650726</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E28" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D28,1)</f>
-        <v>j</v>
+        <v>ro</v>
       </c>
       <c r="F28" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D28,2)</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G28" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -1423,101 +1430,101 @@
       </c>
       <c r="H28" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>604</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4469147.482493869</v>
-      </c>
-      <c r="B29" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5642998.5091750864</v>
-      </c>
-      <c r="C29" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>198.18890480174358</v>
+        <v>528</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A29" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4460110.4834662629</v>
+      </c>
+      <c r="B29" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5659686.9595224261</v>
+      </c>
+      <c r="C29" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>237.00065614631606</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E29" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D29,1)</f>
-        <v>mm</v>
+        <v>d</v>
       </c>
       <c r="F29" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D29,2)</f>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G29" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="H29" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>922</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4473380.553160781</v>
-      </c>
-      <c r="B30" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5654516.1273455229</v>
-      </c>
-      <c r="C30" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>252.57654204834554</v>
+      <c r="H29" s="2" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A30" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4484224.3331929445</v>
+      </c>
+      <c r="B30" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5645390.4754439788</v>
+      </c>
+      <c r="C30" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>319.66643085481718</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E30" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D30,1)</f>
-        <v>sm</v>
+        <v>c</v>
       </c>
       <c r="F30" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D30,2)</f>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G30" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Point Set</v>
+        <v/>
       </c>
       <c r="H30" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4462169.0678236848</v>
-      </c>
-      <c r="B31" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5645696.2819503248</v>
-      </c>
-      <c r="C31" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>236.64143468462601</v>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A31" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4483304.0258460799</v>
+      </c>
+      <c r="B31" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5647052.8566764072</v>
+      </c>
+      <c r="C31" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>259.30881329449397</v>
       </c>
       <c r="D31" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E31" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D31,1)</f>
-        <v>km</v>
+        <v>su</v>
       </c>
       <c r="F31" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D31,2)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="G31" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -1525,33 +1532,33 @@
       </c>
       <c r="H31" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>584</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4514019.3325810712</v>
-      </c>
-      <c r="B32" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5647141.1227576211</v>
-      </c>
-      <c r="C32" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>302.82813839870028</v>
+        <v>551</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A32" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4532147.9670506176</v>
+      </c>
+      <c r="B32" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5642357.4463283438</v>
+      </c>
+      <c r="C32" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>392.99057979059353</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E32" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D32,1)</f>
-        <v>c</v>
+        <v>km</v>
       </c>
       <c r="F32" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D32,2)</f>
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="G32" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
@@ -1562,256 +1569,256 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4542881.4380607037</v>
-      </c>
-      <c r="B33" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5654965.0077083055</v>
-      </c>
-      <c r="C33" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>279.76073849369448</v>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A33" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4450498.3773445711</v>
+      </c>
+      <c r="B33" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5645315.5694493605</v>
+      </c>
+      <c r="C33" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>103.28170325039565</v>
       </c>
       <c r="D33" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E33" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D33,1)</f>
-        <v>z</v>
+        <v>sm</v>
       </c>
       <c r="F33" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D33,2)</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G33" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="H33" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>605</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4514239.1797009064</v>
-      </c>
-      <c r="B34" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5655604.7920794478</v>
-      </c>
-      <c r="C34" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>131.98145333321682</v>
+      <c r="H33" s="2" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A34" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4544464.2791574206</v>
+      </c>
+      <c r="B34" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5643599.2895391146</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>157.58561461688726</v>
       </c>
       <c r="D34" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E34" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D34,1)</f>
-        <v>ro</v>
+        <v>d</v>
       </c>
       <c r="F34" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D34,2)</f>
+        <v>18</v>
+      </c>
+      <c r="G34" s="2" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>Point Set</v>
+      </c>
+      <c r="H34" s="2" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A35" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4529679.2868642332</v>
+      </c>
+      <c r="B35" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5658736.677423723</v>
+      </c>
+      <c r="C35" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>211.59155781986811</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" ca="1" si="3"/>
         <v>15</v>
-      </c>
-      <c r="G34" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Point Set</v>
-      </c>
-      <c r="H34" s="2" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4476697.2062565312</v>
-      </c>
-      <c r="B35" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5647433.9207830867</v>
-      </c>
-      <c r="C35" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>367.98462679775787</v>
-      </c>
-      <c r="D35" s="2">
-        <f t="shared" ca="1" si="3"/>
-        <v>8</v>
       </c>
       <c r="E35" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D35,1)</f>
-        <v>ku</v>
+        <v>z</v>
       </c>
       <c r="F35" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D35,2)</f>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G35" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Point Set</v>
-      </c>
-      <c r="H35" s="2" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4511225.4604298575</v>
-      </c>
-      <c r="B36" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5640436.8242845526</v>
-      </c>
-      <c r="C36" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>418.92265780362868</v>
+        <v/>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" ca="1" si="5"/>
+        <v>558</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4483249.1400776245</v>
+      </c>
+      <c r="B36" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5648086.3336547483</v>
+      </c>
+      <c r="C36" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>413.24266359716523</v>
       </c>
       <c r="D36" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E36" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D36,1)</f>
-        <v>mm</v>
+        <v>j</v>
       </c>
       <c r="F36" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D36,2)</f>
+        <v>4</v>
+      </c>
+      <c r="G36" s="2" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="H36" s="2" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A37" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4511109.0562919406</v>
+      </c>
+      <c r="B37" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5654320.1517166244</v>
+      </c>
+      <c r="C37" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>293.70429908476416</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" ca="1" si="3"/>
         <v>9</v>
-      </c>
-      <c r="G36" s="2" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Point Set</v>
-      </c>
-      <c r="H36" s="2">
-        <f t="shared" ca="1" si="5"/>
-        <v>560</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4534309.2376097599</v>
-      </c>
-      <c r="B37" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5642614.0478889979</v>
-      </c>
-      <c r="C37" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>315.88978821395102</v>
-      </c>
-      <c r="D37" s="2">
-        <f t="shared" ca="1" si="3"/>
-        <v>16</v>
       </c>
       <c r="E37" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D37,1)</f>
-        <v>ro</v>
+        <v>mo</v>
       </c>
       <c r="F37" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D37,2)</f>
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G37" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
         <v>Point Set</v>
       </c>
-      <c r="H37" s="2" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4517680.9853921924</v>
-      </c>
-      <c r="B38" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5640472.3432434322</v>
-      </c>
-      <c r="C38" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>425.63260145436647</v>
+      <c r="H37" s="2">
+        <f t="shared" ca="1" si="5"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A38" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4485708.4809567016</v>
+      </c>
+      <c r="B38" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5649406.7137986459</v>
+      </c>
+      <c r="C38" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>377.87102947161316</v>
       </c>
       <c r="D38" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E38" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D38,1)</f>
-        <v>kr</v>
+        <v>su</v>
       </c>
       <c r="F38" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D38,2)</f>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="G38" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v>Point Set</v>
       </c>
       <c r="H38" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>641</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4453140.278722289</v>
-      </c>
-      <c r="B39" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5657457.1179687195</v>
-      </c>
-      <c r="C39" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>176.44215787867273</v>
+        <v>954</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A39" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4486374.8921940131</v>
+      </c>
+      <c r="B39" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5644624.0817024577</v>
+      </c>
+      <c r="C39" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>237.69169607292264</v>
       </c>
       <c r="D39" s="2">
         <f t="shared" ca="1" si="3"/>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E39" s="2" t="str">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D39,1)</f>
-        <v>mu</v>
+        <v>su</v>
       </c>
       <c r="F39" s="2">
         <f ca="1">INDEX(Stratigraphy!$A$1:$B$20,Randomdata!$D39,2)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G39" s="2" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Point Set</v>
+        <v/>
       </c>
       <c r="H39" s="2" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
-        <f t="shared" ca="1" si="0"/>
-        <v>4544611.1901426129</v>
-      </c>
-      <c r="B40" s="2">
-        <f t="shared" ca="1" si="1"/>
-        <v>5642790.6287891716</v>
-      </c>
-      <c r="C40" s="2">
-        <f t="shared" ca="1" si="2"/>
-        <v>373.56791784552172</v>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A40" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4467016.3354375521</v>
+      </c>
+      <c r="B40" s="4">
+        <f t="shared" ca="1" si="1"/>
+        <v>5657072.8745097537</v>
+      </c>
+      <c r="C40" s="4">
+        <f t="shared" ca="1" si="2"/>
+        <v>411.51741590864947</v>
       </c>
       <c r="D40" s="2">
         <f t="shared" ca="1" si="3"/>
@@ -1848,12 +1855,12 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="13.85546875" style="2" customWidth="1"/>
+    <col min="1" max="2" width="13.86328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1861,7 +1868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1869,7 +1876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1877,7 +1884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1885,7 +1892,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1893,7 +1900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -1901,7 +1908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1909,7 +1916,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1917,7 +1924,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -1925,7 +1932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1933,7 +1940,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1941,7 +1948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1949,7 +1956,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1957,7 +1964,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -1965,7 +1972,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1973,7 +1980,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1981,7 +1988,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -1989,7 +1996,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1997,7 +2004,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -2005,7 +2012,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>

</xml_diff>